<commit_message>
add data insert func from excel file directly
</commit_message>
<xml_diff>
--- a/testworkbook.xlsx
+++ b/testworkbook.xlsx
@@ -2,14 +2,14 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" dateCompatibility="false"/>
+  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId3"/>
-    <sheet name="Sheet2" sheetId="2" state="visible" r:id="rId4"/>
+    <sheet name="parent_dm" sheetId="1" state="visible" r:id="rId3"/>
+    <sheet name="child_dm" sheetId="2" state="visible" r:id="rId4"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -21,47 +21,82 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="20">
   <si>
     <t xml:space="preserve">id</t>
   </si>
   <si>
-    <t xml:space="preserve">test_name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">test_value</t>
-  </si>
-  <si>
-    <t xml:space="preserve">gaq</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ha</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ett</t>
+    <t xml:space="preserve">row_name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">row_desc</t>
+  </si>
+  <si>
+    <t xml:space="preserve">int_val</t>
+  </si>
+  <si>
+    <t xml:space="preserve">decimal_val</t>
+  </si>
+  <si>
+    <t xml:space="preserve">flag</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ONE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">just a desc</t>
+  </si>
+  <si>
+    <t xml:space="preserve">true</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TWO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">THREE</t>
   </si>
   <si>
     <t xml:space="preserve">parent_id</t>
   </si>
   <si>
-    <t xml:space="preserve">int_value</t>
-  </si>
-  <si>
-    <t xml:space="preserve">decimal_value</t>
+    <t xml:space="preserve">child1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">a description</t>
+  </si>
+  <si>
+    <t xml:space="preserve">false</t>
+  </si>
+  <si>
+    <t xml:space="preserve">child2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">child3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">child4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">child5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">child6</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="General"/>
+    <numFmt numFmtId="165" formatCode="@"/>
   </numFmts>
   <fonts count="4">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -121,12 +156,20 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -253,56 +296,92 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C4" activeCellId="0" sqref="C4"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G11" activeCellId="0" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="0" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="n">
+      <c r="A2" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="B2" s="0" t="s">
+      <c r="B2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" s="1" t="n">
+        <v>1000</v>
+      </c>
+      <c r="E2" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" s="1" t="n">
+        <v>2000</v>
+      </c>
+      <c r="E3" s="1" t="n">
+        <v>200</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="C2" s="0" t="n">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="B3" s="0" t="s">
-        <v>4</v>
-      </c>
-      <c r="C3" s="0" t="n">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="B4" s="0" t="s">
-        <v>5</v>
-      </c>
-      <c r="C4" s="0" t="n">
-        <v>45</v>
+      <c r="B4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" s="1" t="n">
+        <v>3000</v>
+      </c>
+      <c r="E4" s="1" t="n">
+        <v>300</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>8</v>
       </c>
     </row>
   </sheetData>
@@ -323,108 +402,108 @@
   </sheetPr>
   <dimension ref="A1:D7"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D7" activeCellId="0" sqref="D7"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E15" activeCellId="0" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="C1" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="D1" s="0" t="s">
+      <c r="A1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3" s="2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="B2" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="C2" s="0" t="n">
-        <v>124</v>
-      </c>
-      <c r="D2" s="0" t="n">
-        <v>12.51</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="n">
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="B3" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="C3" s="0" t="n">
-        <v>123451</v>
-      </c>
-      <c r="D3" s="0" t="n">
-        <v>11.11</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="n">
+      <c r="B4" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="B4" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="C4" s="0" t="n">
-        <v>532</v>
-      </c>
-      <c r="D4" s="1" t="n">
-        <v>32.54</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="n">
-        <v>4</v>
-      </c>
-      <c r="B5" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="C5" s="0" t="n">
-        <v>21</v>
-      </c>
-      <c r="D5" s="0" t="n">
-        <v>44.21</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="n">
-        <v>5</v>
-      </c>
-      <c r="B6" s="0" t="n">
+      <c r="B6" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="C6" s="0" t="n">
-        <v>45</v>
-      </c>
-      <c r="D6" s="0" t="n">
-        <v>6433.253</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="n">
-        <v>6</v>
-      </c>
-      <c r="B7" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="C7" s="0" t="n">
-        <v>11</v>
-      </c>
-      <c r="D7" s="0" t="n">
-        <v>2.1</v>
+      <c r="B7" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>